<commit_message>
Quick correction of years in investment cost excel
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
@@ -1,21 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEB54C6-74C1-4119-9ED3-44BA168EF897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{3DEB54C6-74C1-4119-9ED3-44BA168EF897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5199D2D1-64DD-42E3-87AE-D4ABCCCEFDCF}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
+    <workbookView xWindow="-22215" yWindow="-20550" windowWidth="27570" windowHeight="14460" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
   </bookViews>
   <sheets>
     <sheet name="Investment_Cost" sheetId="1" r:id="rId1"/>
     <sheet name="Sources" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="CIQWBGuid" hidden="1">"2f1f32c2-b0bb-4653-88c7-8313657ec4b2"</definedName>
+    <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
+    <definedName name="IQ_CH">110000</definedName>
+    <definedName name="IQ_CQ">5000</definedName>
+    <definedName name="IQ_CY">10000</definedName>
+    <definedName name="IQ_DAILY">500000</definedName>
+    <definedName name="IQ_DNTM" hidden="1">700000</definedName>
+    <definedName name="IQ_FH">100000</definedName>
+    <definedName name="IQ_FQ">500</definedName>
+    <definedName name="IQ_FWD_CY" hidden="1">10001</definedName>
+    <definedName name="IQ_FWD_CY1" hidden="1">10002</definedName>
+    <definedName name="IQ_FWD_CY2" hidden="1">10003</definedName>
+    <definedName name="IQ_FWD_FY" hidden="1">1001</definedName>
+    <definedName name="IQ_FWD_FY1" hidden="1">1002</definedName>
+    <definedName name="IQ_FWD_FY2" hidden="1">1003</definedName>
+    <definedName name="IQ_FWD_Q" hidden="1">501</definedName>
+    <definedName name="IQ_FWD_Q1" hidden="1">502</definedName>
+    <definedName name="IQ_FWD_Q2" hidden="1">503</definedName>
+    <definedName name="IQ_FY">1000</definedName>
+    <definedName name="IQ_LATESTK" hidden="1">1000</definedName>
+    <definedName name="IQ_LATESTQ" hidden="1">500</definedName>
+    <definedName name="IQ_LTM">2000</definedName>
+    <definedName name="IQ_LTMMONTH" hidden="1">120000</definedName>
+    <definedName name="IQ_MONTH">15000</definedName>
+    <definedName name="IQ_MTD" hidden="1">800000</definedName>
+    <definedName name="IQ_NAMES_REVISION_DATE_" hidden="1">45429.7589699074</definedName>
+    <definedName name="IQ_NTM">6000</definedName>
+    <definedName name="IQ_QTD" hidden="1">750000</definedName>
+    <definedName name="IQ_TODAY" hidden="1">0</definedName>
+    <definedName name="IQ_WEEK">50000</definedName>
+    <definedName name="IQ_YTD">3000</definedName>
+    <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>PV_plant</t>
   </si>
@@ -73,6 +107,18 @@
   </si>
   <si>
     <t>Hydrogen_storage</t>
+  </si>
+  <si>
+    <t>Investment_Cost [Euro/MW or MWh] Value 2025</t>
+  </si>
+  <si>
+    <t>Investment_Cost [Euro/MW or MWh] Value 2030</t>
+  </si>
+  <si>
+    <t>Investment_Cost [Euro/MW or MWh] Value 2040</t>
+  </si>
+  <si>
+    <t>Investment_Cost [Euro/MW or MWh] Value 2050</t>
   </si>
 </sst>
 </file>
@@ -463,17 +509,17 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="6" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="6" width="15.54296875" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -481,19 +527,19 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -513,7 +559,7 @@
         <v>290000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -533,7 +579,7 @@
         <v>475000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -553,7 +599,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -573,7 +619,7 @@
         <v>800000</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -593,7 +639,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -614,7 +660,7 @@
       </c>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -634,7 +680,7 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -654,7 +700,7 @@
         <v>1.3958682300390843E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -684,13 +730,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262416F5-07F9-4A10-AA36-6136A8834922}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Renamed model data bases + electrolyzer names
Electrolyzer_PEM -> PEM_Electrolyzer for matching investment costs
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{3DEB54C6-74C1-4119-9ED3-44BA168EF897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5199D2D1-64DD-42E3-87AE-D4ABCCCEFDCF}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{3DEB54C6-74C1-4119-9ED3-44BA168EF897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDE79035-A84F-400E-9F1F-B01748EB4E1A}"/>
   <bookViews>
-    <workbookView xWindow="-22215" yWindow="-20550" windowWidth="27570" windowHeight="14460" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
+    <workbookView xWindow="-22815" yWindow="-21720" windowWidth="51840" windowHeight="21240" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
   </bookViews>
   <sheets>
     <sheet name="Investment_Cost" sheetId="1" r:id="rId1"/>
     <sheet name="Sources" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"2f1f32c2-b0bb-4653-88c7-8313657ec4b2"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"35c1342b-6740-40cd-b152-b55cc00a54f4"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -94,15 +94,6 @@
     <t>Electric_Steam_Boiler</t>
   </si>
   <si>
-    <t>Electrolyzer_AEC</t>
-  </si>
-  <si>
-    <t>Electrolyzer_PEM</t>
-  </si>
-  <si>
-    <t>Electrolyzer_SOEC</t>
-  </si>
-  <si>
     <t>Methanol_storage</t>
   </si>
   <si>
@@ -119,6 +110,15 @@
   </si>
   <si>
     <t>Investment_Cost [Euro/MW or MWh] Value 2050</t>
+  </si>
+  <si>
+    <t>AEC_Electrolyzer</t>
+  </si>
+  <si>
+    <t>PEM_Electrolyzer</t>
+  </si>
+  <si>
+    <t>SOEC_Electrolyzer</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -527,16 +527,16 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -561,7 +561,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3">
         <v>1900000</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3">
         <v>1900000</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3">
         <v>2900000</v>
@@ -682,7 +682,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3">
         <v>1.3958682300390843E-4</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>0.121</v>

</xml_diff>

<commit_message>
Changed investment structure + fixed problems
To reduce redundancy I moved all lifetimes and costs to the investment overview excel
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{3DEB54C6-74C1-4119-9ED3-44BA168EF897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D79D0E5E-BF9B-48F6-8217-007AB0B5870C}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:1_{3DEB54C6-74C1-4119-9ED3-44BA168EF897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{250E1D65-0566-477A-9F5B-ADB7147AB7AD}"/>
   <bookViews>
-    <workbookView xWindow="-22815" yWindow="-21720" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
   </bookViews>
   <sheets>
     <sheet name="Investment_Cost" sheetId="1" r:id="rId1"/>
     <sheet name="Sources" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"0ead5223-d2e4-413b-a47b-346b57e8674b"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"1893ca4e-b437-4a66-b598-08d6c7ee1d1f"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>PV_plant</t>
   </si>
@@ -121,7 +121,31 @@
     <t>SOEC_Electrolyzer</t>
   </si>
   <si>
-    <t>Wind_farm</t>
+    <t>Wind_onshore</t>
+  </si>
+  <si>
+    <t>Wind_offshore</t>
+  </si>
+  <si>
+    <t>Lifetime</t>
+  </si>
+  <si>
+    <t>35Y</t>
+  </si>
+  <si>
+    <t>25Y</t>
+  </si>
+  <si>
+    <t>20Y</t>
+  </si>
+  <si>
+    <t>Destilation_tower</t>
+  </si>
+  <si>
+    <t>30Y</t>
+  </si>
+  <si>
+    <t>27Y</t>
   </si>
 </sst>
 </file>
@@ -168,13 +192,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FABD746-4A8E-4371-B5EF-19107F5A398A}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,125 +566,146 @@
       <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>560000</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>560000</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>380000</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>320000</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <v>290000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>1900000</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>1400000</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>875000</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>675000</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <v>475000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>1900000</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>1425000</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>950000</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <v>725000</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="4">
         <v>500000</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>2900000</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>2075000</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>1250000</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>1050000</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="4">
         <v>800000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>500000</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>500000</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <v>500000</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <v>500000</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="4">
         <v>500000</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>1350000</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>1350000</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <v>1090000</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>960000</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="4">
         <v>870000</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
       </c>
       <c r="I7" s="3"/>
     </row>
@@ -667,20 +713,23 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="4">
         <v>150000</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <v>145000.00000000003</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="4">
         <v>140000</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="4">
         <v>135000</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="4">
         <v>130000</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -702,6 +751,9 @@
       <c r="F9" s="3">
         <v>1.3958682300390843E-4</v>
       </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -722,25 +774,77 @@
       <c r="F10" s="3">
         <v>4.5999999999999999E-2</v>
       </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3">
-        <v>1920000</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1920000</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="B11" s="4">
+        <v>1110000</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1180000</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1150000</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1110000</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1090000</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="4">
+        <v>2120000</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1880000</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1800000</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1680000</v>
+      </c>
+      <c r="F12" s="4">
         <v>1640000</v>
       </c>
-      <c r="E11" s="3">
-        <v>1640000</v>
-      </c>
-      <c r="F11" s="3">
-        <v>1390000</v>
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1350000</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1350000</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1090000</v>
+      </c>
+      <c r="E13" s="4">
+        <v>960000</v>
+      </c>
+      <c r="F13" s="4">
+        <v>870000</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -753,7 +857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262416F5-07F9-4A10-AA36-6136A8834922}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adjustment of investement cost calculations
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:1_{3DEB54C6-74C1-4119-9ED3-44BA168EF897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{250E1D65-0566-477A-9F5B-ADB7147AB7AD}"/>
@@ -537,7 +537,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Update for "distillation" tower + beginnings of abbreviations
pipeline/powerline -> PL
Ran for 3 days without problems, will conduct further tests now.
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:1_{3DEB54C6-74C1-4119-9ED3-44BA168EF897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{250E1D65-0566-477A-9F5B-ADB7147AB7AD}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="13_ncr:1_{3DEB54C6-74C1-4119-9ED3-44BA168EF897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CF49EA4-A893-4D50-814C-9F28EAA02E2E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
   </bookViews>
@@ -139,13 +139,13 @@
     <t>20Y</t>
   </si>
   <si>
-    <t>Destilation_tower</t>
-  </si>
-  <si>
     <t>30Y</t>
   </si>
   <si>
     <t>27Y</t>
+  </si>
+  <si>
+    <t>Distillation_tower</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -705,7 +705,7 @@
         <v>870000</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I7" s="3"/>
     </row>
@@ -798,7 +798,7 @@
         <v>1090000</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -821,12 +821,12 @@
         <v>1640000</v>
       </c>
       <c r="G12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4">
         <v>1350000</v>
@@ -844,7 +844,7 @@
         <v>870000</v>
       </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update cost parameter values
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\investment_cost_overview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="13_ncr:1_{3DEB54C6-74C1-4119-9ED3-44BA168EF897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CF49EA4-A893-4D50-814C-9F28EAA02E2E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040390BF-2FAC-42BB-B884-8F7F0DD5CB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
+    <workbookView xWindow="-4590" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
   </bookViews>
   <sheets>
     <sheet name="Investment_Cost" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>PV_plant</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Distillation_tower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The methanol plant value is set to 1 to give the model a cost. The investment itself is in the distillation tower for the output of methanol. </t>
   </si>
 </sst>
 </file>
@@ -192,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -200,6 +203,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FABD746-4A8E-4371-B5EF-19107F5A398A}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -690,19 +694,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="4">
-        <v>1350000</v>
+        <v>1</v>
       </c>
       <c r="C7" s="4">
-        <v>1350000</v>
+        <v>1</v>
       </c>
       <c r="D7" s="4">
-        <v>1090000</v>
+        <v>1</v>
       </c>
       <c r="E7" s="4">
-        <v>960000</v>
+        <v>1</v>
       </c>
       <c r="F7" s="4">
-        <v>870000</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
         <v>22</v>
@@ -737,19 +741,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>1.3958682300390843E-4</v>
+        <v>139.58682300390799</v>
       </c>
       <c r="C9" s="3">
-        <v>1.3958682300390843E-4</v>
+        <v>139.58682300390799</v>
       </c>
       <c r="D9" s="3">
-        <v>1.3958682300390843E-4</v>
+        <v>139.58682300390799</v>
       </c>
       <c r="E9" s="3">
-        <v>1.3958682300390843E-4</v>
+        <v>139.58682300390799</v>
       </c>
       <c r="F9" s="3">
-        <v>1.3958682300390843E-4</v>
+        <v>139.58682300390799</v>
       </c>
       <c r="G9" t="s">
         <v>20</v>
@@ -759,20 +763,20 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
-        <v>0.121</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.17049999999999998</v>
-      </c>
-      <c r="D10" s="3">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="E10" s="3">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="F10" s="3">
-        <v>4.5999999999999999E-2</v>
+      <c r="B10" s="4">
+        <v>121000</v>
+      </c>
+      <c r="C10" s="4">
+        <v>170500</v>
+      </c>
+      <c r="D10" s="4">
+        <v>99000</v>
+      </c>
+      <c r="E10" s="4">
+        <v>61000</v>
+      </c>
+      <c r="F10" s="4">
+        <v>46000</v>
       </c>
       <c r="G10" t="s">
         <v>20</v>
@@ -846,6 +850,12 @@
       <c r="G13" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -855,10 +865,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262416F5-07F9-4A10-AA36-6136A8834922}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -868,6 +878,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update investment cost input sheet
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\investment_cost_overview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040390BF-2FAC-42BB-B884-8F7F0DD5CB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47FB6F8-5F79-40D1-9861-B8828A889F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4590" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
   </bookViews>
   <sheets>
     <sheet name="Investment_Cost" sheetId="1" r:id="rId1"/>
@@ -541,7 +541,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -767,7 +767,7 @@
         <v>121000</v>
       </c>
       <c r="C10" s="4">
-        <v>170500</v>
+        <v>110000</v>
       </c>
       <c r="D10" s="4">
         <v>99000</v>

</xml_diff>

<commit_message>
Added fom cost percentage to inv overview
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{B47FB6F8-5F79-40D1-9861-B8828A889F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4852EA89-412F-488F-B87E-DE9EA71F272B}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{B47FB6F8-5F79-40D1-9861-B8828A889F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B9E969F-4867-4875-B9AB-0CF20BBB3F8E}"/>
   <bookViews>
-    <workbookView xWindow="-13200" yWindow="-16275" windowWidth="14400" windowHeight="7365" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
+    <workbookView xWindow="-10515" yWindow="-18810" windowWidth="28800" windowHeight="14595" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
   </bookViews>
   <sheets>
     <sheet name="Investment_Cost" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>PV_plant</t>
   </si>
@@ -149,16 +149,19 @@
   </si>
   <si>
     <t xml:space="preserve">The methanol plant value is set to 1 to give the model a cost. The investment itself is in the distillation tower for the output of methanol. </t>
+  </si>
+  <si>
+    <t>fom_cost_share</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +171,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -192,10 +202,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -204,12 +215,81 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{929C245B-1C98-42F4-86C0-4126092245FE}">
+      <tableStyleElement type="secondColumnStripe" dxfId="2"/>
+    </tableStyle>
+    <tableStyle name="Table Style 2" pivot="0" count="2" xr9:uid="{BBAF72AA-9687-4D85-A8FB-DD10D4A3A7DE}">
+      <tableStyleElement type="headerRow" dxfId="1"/>
+      <tableStyleElement type="firstRowStripe" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -223,6 +303,23 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{444AF12D-6150-4645-AFF5-4209C0C8ABE5}" name="Table1" displayName="Table1" ref="A1:H24" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:H24" xr:uid="{444AF12D-6150-4645-AFF5-4209C0C8ABE5}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{1C0839C7-21FD-4A7F-9467-95BCDFF1A4EB}" name="Object_type"/>
+    <tableColumn id="2" xr3:uid="{C545414A-8E96-4DD0-B69F-C2864283FDB2}" name="Investment_Cost [Euro/MW or MWh] Value 2020" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{C6660AE0-993C-48C6-BFE7-4B992D75C3DC}" name="Investment_Cost [Euro/MW or MWh] Value 2025" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{5823E4EA-55C9-4AD7-AEBF-43B1401D5856}" name="Investment_Cost [Euro/MW or MWh] Value 2030" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{9CB82FB8-8E5F-41F3-A4E2-B16ACB85D740}" name="Investment_Cost [Euro/MW or MWh] Value 2040" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{F1AACD89-09D9-4BEE-96AA-01889149FFEF}" name="Investment_Cost [Euro/MW or MWh] Value 2050" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{AD0B09D5-EE54-4534-89C9-CF7E377065D8}" name="Lifetime"/>
+    <tableColumn id="8" xr3:uid="{18F4CB86-F3E7-451B-B7B9-4E2DDB3820E2}" name="fom_cost_share" dataCellStyle="Percent"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -544,18 +641,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FABD746-4A8E-4371-B5EF-19107F5A398A}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="6" width="15.54296875" customWidth="1"/>
+    <col min="2" max="6" width="32.26953125" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" customWidth="1"/>
+    <col min="8" max="8" width="16.54296875" customWidth="1"/>
     <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -576,6 +673,9 @@
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -600,6 +700,9 @@
       <c r="G2" t="s">
         <v>19</v>
       </c>
+      <c r="H2" s="6">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -623,6 +726,9 @@
       <c r="G3" t="s">
         <v>20</v>
       </c>
+      <c r="H3" s="6">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -646,6 +752,9 @@
       <c r="G4" t="s">
         <v>20</v>
       </c>
+      <c r="H4" s="6">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -669,6 +778,9 @@
       <c r="G5" t="s">
         <v>20</v>
       </c>
+      <c r="H5" s="6">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -692,6 +804,9 @@
       <c r="G6" t="s">
         <v>21</v>
       </c>
+      <c r="H6" s="6">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -715,6 +830,9 @@
       <c r="G7" t="s">
         <v>22</v>
       </c>
+      <c r="H7" s="6">
+        <v>0.02</v>
+      </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -739,6 +857,9 @@
       <c r="G8" t="s">
         <v>21</v>
       </c>
+      <c r="H8" s="6">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -762,6 +883,9 @@
       <c r="G9" t="s">
         <v>20</v>
       </c>
+      <c r="H9" s="6">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -785,6 +909,9 @@
       <c r="G10" t="s">
         <v>20</v>
       </c>
+      <c r="H10" s="6">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -808,6 +935,9 @@
       <c r="G11" t="s">
         <v>23</v>
       </c>
+      <c r="H11" s="6">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -831,6 +961,9 @@
       <c r="G12" t="s">
         <v>23</v>
       </c>
+      <c r="H12" s="6">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -854,16 +987,107 @@
       <c r="G13" t="s">
         <v>22</v>
       </c>
+      <c r="H13" s="6">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" s="4"/>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="E26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated Investment costs and availabilities of price zones
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{B47FB6F8-5F79-40D1-9861-B8828A889F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B9E969F-4867-4875-B9AB-0CF20BBB3F8E}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="114_{03ECC47D-01C7-46E7-B6C9-E689C45291DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2072921E-8C2B-44C5-A882-310444981474}"/>
   <bookViews>
-    <workbookView xWindow="-10515" yWindow="-18810" windowWidth="28800" windowHeight="14595" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
   </bookViews>
   <sheets>
     <sheet name="Investment_Cost" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>PV_plant</t>
   </si>
@@ -152,6 +152,42 @@
   </si>
   <si>
     <t>fom_cost_share</t>
+  </si>
+  <si>
+    <t>Fischer_Tropsch_Unit</t>
+  </si>
+  <si>
+    <t>RWGS_Unit</t>
+  </si>
+  <si>
+    <t>Distillation_tower_FT</t>
+  </si>
+  <si>
+    <t>ASU</t>
+  </si>
+  <si>
+    <t>Haber_Bosch_Reactor</t>
+  </si>
+  <si>
+    <t>Methane_Plant</t>
+  </si>
+  <si>
+    <t>Digester</t>
+  </si>
+  <si>
+    <t>CO2_Remover</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Percentage not specifically given</t>
+  </si>
+  <si>
+    <t>No value given for 2025 (linearly approximated)</t>
+  </si>
+  <si>
+    <t>Inv_costs calculated using percentage from catalogue (see data_needed)</t>
   </si>
 </sst>
 </file>
@@ -206,7 +242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -216,35 +252,17 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.89996032593768116"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.89996032593768116"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
@@ -280,14 +298,38 @@
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{929C245B-1C98-42F4-86C0-4126092245FE}">
-      <tableStyleElement type="secondColumnStripe" dxfId="2"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="9"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="2" xr9:uid="{BBAF72AA-9687-4D85-A8FB-DD10D4A3A7DE}">
-      <tableStyleElement type="headerRow" dxfId="1"/>
-      <tableStyleElement type="firstRowStripe" dxfId="0"/>
+      <tableStyleElement type="headerRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -301,22 +343,19 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{444AF12D-6150-4645-AFF5-4209C0C8ABE5}" name="Table1" displayName="Table1" ref="A1:H24" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:H24" xr:uid="{444AF12D-6150-4645-AFF5-4209C0C8ABE5}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{444AF12D-6150-4645-AFF5-4209C0C8ABE5}" name="Table1" displayName="Table1" ref="A1:I24" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:I24" xr:uid="{444AF12D-6150-4645-AFF5-4209C0C8ABE5}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{1C0839C7-21FD-4A7F-9467-95BCDFF1A4EB}" name="Object_type"/>
-    <tableColumn id="2" xr3:uid="{C545414A-8E96-4DD0-B69F-C2864283FDB2}" name="Investment_Cost [Euro/MW or MWh] Value 2020" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{C6660AE0-993C-48C6-BFE7-4B992D75C3DC}" name="Investment_Cost [Euro/MW or MWh] Value 2025" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{5823E4EA-55C9-4AD7-AEBF-43B1401D5856}" name="Investment_Cost [Euro/MW or MWh] Value 2030" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{9CB82FB8-8E5F-41F3-A4E2-B16ACB85D740}" name="Investment_Cost [Euro/MW or MWh] Value 2040" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{F1AACD89-09D9-4BEE-96AA-01889149FFEF}" name="Investment_Cost [Euro/MW or MWh] Value 2050" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{C545414A-8E96-4DD0-B69F-C2864283FDB2}" name="Investment_Cost [Euro/MW or MWh] Value 2020" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{C6660AE0-993C-48C6-BFE7-4B992D75C3DC}" name="Investment_Cost [Euro/MW or MWh] Value 2025" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{5823E4EA-55C9-4AD7-AEBF-43B1401D5856}" name="Investment_Cost [Euro/MW or MWh] Value 2030" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{9CB82FB8-8E5F-41F3-A4E2-B16ACB85D740}" name="Investment_Cost [Euro/MW or MWh] Value 2040" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{F1AACD89-09D9-4BEE-96AA-01889149FFEF}" name="Investment_Cost [Euro/MW or MWh] Value 2050" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{AD0B09D5-EE54-4534-89C9-CF7E377065D8}" name="Lifetime"/>
     <tableColumn id="8" xr3:uid="{18F4CB86-F3E7-451B-B7B9-4E2DDB3820E2}" name="fom_cost_share" dataCellStyle="Percent"/>
+    <tableColumn id="9" xr3:uid="{AB438110-8B80-474F-9085-9A01BC3E4DFF}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -641,7 +680,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FABD746-4A8E-4371-B5EF-19107F5A398A}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -649,7 +690,7 @@
     <col min="2" max="6" width="32.26953125" customWidth="1"/>
     <col min="7" max="7" width="10.08984375" customWidth="1"/>
     <col min="8" max="8" width="16.54296875" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -677,6 +718,9 @@
       <c r="H1" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -703,6 +747,7 @@
       <c r="H2" s="6">
         <v>0.02</v>
       </c>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -729,6 +774,7 @@
       <c r="H3" s="6">
         <v>0.02</v>
       </c>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -755,6 +801,7 @@
       <c r="H4" s="6">
         <v>0.02</v>
       </c>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -781,6 +828,7 @@
       <c r="H5" s="6">
         <v>0.02</v>
       </c>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -807,6 +855,7 @@
       <c r="H6" s="6">
         <v>0.02</v>
       </c>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -833,7 +882,7 @@
       <c r="H7" s="6">
         <v>0.02</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -860,6 +909,7 @@
       <c r="H8" s="6">
         <v>0.02</v>
       </c>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -886,6 +936,7 @@
       <c r="H9" s="6">
         <v>0.02</v>
       </c>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -912,6 +963,7 @@
       <c r="H10" s="6">
         <v>0.02</v>
       </c>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -938,6 +990,7 @@
       <c r="H11" s="6">
         <v>0.02</v>
       </c>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -964,6 +1017,7 @@
       <c r="H12" s="6">
         <v>0.02</v>
       </c>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -990,96 +1044,260 @@
       <c r="H13" s="6">
         <v>0.02</v>
       </c>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="H14" s="6"/>
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2100000</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1850000</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1600000</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1100000</v>
+      </c>
+      <c r="F14" s="7">
+        <v>900000</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="H15" s="6"/>
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="4">
+        <v>413513.5</v>
+      </c>
+      <c r="C17" s="4">
+        <v>377027</v>
+      </c>
+      <c r="D17" s="4">
+        <v>340540.5</v>
+      </c>
+      <c r="E17" s="4">
+        <v>267567.59999999998</v>
+      </c>
+      <c r="F17" s="4">
+        <v>218567.6</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1700000</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1550000</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1400000</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1100000</v>
+      </c>
+      <c r="F18" s="4">
+        <v>900000</v>
+      </c>
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="4">
+        <v>9600000</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2100000</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1500000</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="G19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="H22" s="6"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="H24" s="6"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I24" s="4"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E26" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renaming and location change of availabilty sheets
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="114_{03ECC47D-01C7-46E7-B6C9-E689C45291DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2072921E-8C2B-44C5-A882-310444981474}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="114_{03ECC47D-01C7-46E7-B6C9-E689C45291DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA409B45-FCE8-46E0-8D13-54EF9229813C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>PV_plant</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Inv_costs calculated using percentage from catalogue (see data_needed)</t>
+  </si>
+  <si>
+    <t>No value given for 2025 (linear approximated)</t>
   </si>
 </sst>
 </file>
@@ -680,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FABD746-4A8E-4371-B5EF-19107F5A398A}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1051,19 +1054,19 @@
         <v>27</v>
       </c>
       <c r="B14" s="4">
-        <v>2100000</v>
+        <v>2233000</v>
       </c>
       <c r="C14" s="4">
-        <v>1850000</v>
+        <v>1967000</v>
       </c>
       <c r="D14" s="4">
-        <v>1600000</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1100000</v>
+        <v>1701000</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1170000</v>
       </c>
       <c r="F14" s="7">
-        <v>900000</v>
+        <v>957000</v>
       </c>
       <c r="G14" t="s">
         <v>20</v>
@@ -1072,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
added investment costs for ammonia and diesel storage
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="114_{03ECC47D-01C7-46E7-B6C9-E689C45291DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF6289B2-02B5-4987-9750-C22693E15F8C}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="114_{03ECC47D-01C7-46E7-B6C9-E689C45291DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CCC44E9-49A7-441D-9D8D-87BC7F8F783E}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="-20895" windowWidth="25020" windowHeight="19680" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
   </bookViews>
   <sheets>
     <sheet name="Investment_Cost" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>PV_plant</t>
   </si>
@@ -203,6 +203,27 @@
   </si>
   <si>
     <t>Methane_storage</t>
+  </si>
+  <si>
+    <t>Ammonia_storage</t>
+  </si>
+  <si>
+    <t>Costs are for 2010 but book is from 2024 so these are probably still relevant, Tanks are either pressurized or refrigerated so power supply needed (https://www.sciencedirect.com/science/article/pii/B9780323885164000111)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ammonia storage: </t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/B9780323885164000111, Figure 11.4</t>
+  </si>
+  <si>
+    <t>Diesel storage:</t>
+  </si>
+  <si>
+    <t>https://thundersaidenergy.com/downloads/storage-tank-costs-storing-oil-energy-water-and-chemicals/</t>
+  </si>
+  <si>
+    <t>Average value taken from chart and calculated from $/L to €/MWh using the energy density</t>
   </si>
 </sst>
 </file>
@@ -212,7 +233,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +256,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -253,11 +282,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -265,17 +295,56 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="17">
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
@@ -340,11 +409,11 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{929C245B-1C98-42F4-86C0-4126092245FE}">
-      <tableStyleElement type="secondColumnStripe" dxfId="9"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="16"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="2" xr9:uid="{BBAF72AA-9687-4D85-A8FB-DD10D4A3A7DE}">
-      <tableStyleElement type="headerRow" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -358,19 +427,23 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{444AF12D-6150-4645-AFF5-4209C0C8ABE5}" name="Table1" displayName="Table1" ref="A1:I25" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:I25" xr:uid="{444AF12D-6150-4645-AFF5-4209C0C8ABE5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{444AF12D-6150-4645-AFF5-4209C0C8ABE5}" name="Table1" displayName="Table1" ref="A1:I29" totalsRowCount="1" headerRowDxfId="13">
+  <autoFilter ref="A1:I28" xr:uid="{444AF12D-6150-4645-AFF5-4209C0C8ABE5}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{1C0839C7-21FD-4A7F-9467-95BCDFF1A4EB}" name="Object_type"/>
-    <tableColumn id="2" xr3:uid="{C545414A-8E96-4DD0-B69F-C2864283FDB2}" name="Investment_Cost [Euro/MW or MWh] Value 2020" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{C6660AE0-993C-48C6-BFE7-4B992D75C3DC}" name="Investment_Cost [Euro/MW or MWh] Value 2025" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{5823E4EA-55C9-4AD7-AEBF-43B1401D5856}" name="Investment_Cost [Euro/MW or MWh] Value 2030" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{9CB82FB8-8E5F-41F3-A4E2-B16ACB85D740}" name="Investment_Cost [Euro/MW or MWh] Value 2040" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{F1AACD89-09D9-4BEE-96AA-01889149FFEF}" name="Investment_Cost [Euro/MW or MWh] Value 2050" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{C545414A-8E96-4DD0-B69F-C2864283FDB2}" name="Investment_Cost [Euro/MW or MWh] Value 2020" dataDxfId="12" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{C6660AE0-993C-48C6-BFE7-4B992D75C3DC}" name="Investment_Cost [Euro/MW or MWh] Value 2025" dataDxfId="11" totalsRowDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{5823E4EA-55C9-4AD7-AEBF-43B1401D5856}" name="Investment_Cost [Euro/MW or MWh] Value 2030" dataDxfId="10" totalsRowDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{9CB82FB8-8E5F-41F3-A4E2-B16ACB85D740}" name="Investment_Cost [Euro/MW or MWh] Value 2040" dataDxfId="9" totalsRowDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{F1AACD89-09D9-4BEE-96AA-01889149FFEF}" name="Investment_Cost [Euro/MW or MWh] Value 2050" dataDxfId="8" totalsRowDxfId="2"/>
     <tableColumn id="7" xr3:uid="{AD0B09D5-EE54-4534-89C9-CF7E377065D8}" name="Lifetime"/>
-    <tableColumn id="8" xr3:uid="{18F4CB86-F3E7-451B-B7B9-4E2DDB3820E2}" name="fom_cost_share" dataCellStyle="Percent"/>
-    <tableColumn id="9" xr3:uid="{AB438110-8B80-474F-9085-9A01BC3E4DFF}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{18F4CB86-F3E7-451B-B7B9-4E2DDB3820E2}" name="fom_cost_share" totalsRowDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="9" xr3:uid="{AB438110-8B80-474F-9085-9A01BC3E4DFF}" name="Notes" dataDxfId="7" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -693,9 +766,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FABD746-4A8E-4371-B5EF-19107F5A398A}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -757,7 +832,7 @@
       <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>0.02</v>
       </c>
       <c r="I2" s="4"/>
@@ -784,7 +859,7 @@
       <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>0.02</v>
       </c>
       <c r="I3" s="4"/>
@@ -811,7 +886,7 @@
       <c r="G4" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>0.02</v>
       </c>
       <c r="I4" s="4"/>
@@ -838,7 +913,7 @@
       <c r="G5" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>0.02</v>
       </c>
       <c r="I5" s="4"/>
@@ -865,7 +940,7 @@
       <c r="G6" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>0.02</v>
       </c>
       <c r="I6" s="4"/>
@@ -884,7 +959,7 @@
       <c r="G7" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>0.02</v>
       </c>
       <c r="I7" s="4"/>
@@ -911,7 +986,7 @@
       <c r="G8" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>0.02</v>
       </c>
       <c r="I8" s="4"/>
@@ -938,7 +1013,7 @@
       <c r="G9" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>0.02</v>
       </c>
       <c r="I9" s="4"/>
@@ -965,7 +1040,7 @@
       <c r="G10" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>0.02</v>
       </c>
       <c r="I10" s="4"/>
@@ -992,7 +1067,7 @@
       <c r="G11" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>0.02</v>
       </c>
       <c r="I11" s="4"/>
@@ -1019,7 +1094,7 @@
       <c r="G12" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>0.02</v>
       </c>
       <c r="I12" s="4"/>
@@ -1046,7 +1121,7 @@
       <c r="G13" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>0.02</v>
       </c>
       <c r="I13" s="4"/>
@@ -1064,16 +1139,16 @@
       <c r="D14" s="4">
         <v>1701000</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>1170000</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>957000</v>
       </c>
       <c r="G14" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <v>0</v>
       </c>
       <c r="I14" s="4" t="s">
@@ -1102,7 +1177,7 @@
       <c r="G15" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <v>0</v>
       </c>
       <c r="I15" s="4"/>
@@ -1129,7 +1204,7 @@
       <c r="G16" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <v>0</v>
       </c>
       <c r="I16" s="4"/>
@@ -1156,7 +1231,7 @@
       <c r="G17" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <v>0.03</v>
       </c>
       <c r="I17" s="4" t="s">
@@ -1185,7 +1260,7 @@
       <c r="G18" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <v>0.03</v>
       </c>
       <c r="I18" s="4" t="s">
@@ -1214,7 +1289,7 @@
       <c r="G19" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <v>0.03</v>
       </c>
       <c r="I19" s="4" t="s">
@@ -1243,7 +1318,7 @@
       <c r="G20" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="5">
         <v>0.03</v>
       </c>
       <c r="I20" s="4"/>
@@ -1270,7 +1345,7 @@
       <c r="G21" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="5">
         <v>0.03</v>
       </c>
       <c r="I21" s="4"/>
@@ -1279,13 +1354,27 @@
       <c r="A22" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="4"/>
+      <c r="B22" s="4">
+        <v>25</v>
+      </c>
+      <c r="C22" s="4">
+        <v>25</v>
+      </c>
+      <c r="D22" s="4">
+        <v>25</v>
+      </c>
+      <c r="E22" s="4">
+        <v>25</v>
+      </c>
+      <c r="F22" s="4">
+        <v>25</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -1296,7 +1385,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="H23" s="6"/>
+      <c r="H23" s="5"/>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -1308,7 +1397,7 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="H24" s="6"/>
+      <c r="H24" s="5"/>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -1320,11 +1409,59 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="H25" s="6"/>
+      <c r="H25" s="5"/>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E26" s="5"/>
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="4">
+        <v>4400</v>
+      </c>
+      <c r="C26" s="4">
+        <v>4400</v>
+      </c>
+      <c r="D26" s="4">
+        <v>4400</v>
+      </c>
+      <c r="E26" s="4">
+        <v>4400</v>
+      </c>
+      <c r="F26" s="4">
+        <v>4400</v>
+      </c>
+      <c r="H26" s="5"/>
+      <c r="I26" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1337,25 +1474,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262416F5-07F9-4A10-AA36-6136A8834922}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>25</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{64D3313F-6197-4079-A3A9-6D968C141F9B}"/>
+    <hyperlink ref="C7" r:id="rId2" xr:uid="{1F6F963B-5D7A-4687-B8FB-910A57C1D205}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Capacity + Inv limit fix
Changed code such that capacity values and investment values shown in interface are the actual values used instead of placeholder values
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="114_{03ECC47D-01C7-46E7-B6C9-E689C45291DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CCC44E9-49A7-441D-9D8D-87BC7F8F783E}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="114_{03ECC47D-01C7-46E7-B6C9-E689C45291DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{138869CC-AA2B-499E-A164-B65191E9F22F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
   </bookViews>
   <sheets>
     <sheet name="Investment_Cost" sheetId="1" r:id="rId1"/>
@@ -300,7 +300,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -312,22 +312,6 @@
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
@@ -425,10 +409,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -768,9 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FABD746-4A8E-4371-B5EF-19107F5A398A}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -949,10 +927,18 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
       <c r="F7" s="4">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Power Storage Investment Option
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/investment_cost_overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\investment_cost_overview\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/investment_cost_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0F3777-73D1-41BF-80D4-5E66D841CD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{6D0F3777-73D1-41BF-80D4-5E66D841CD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A7A42DF-DD73-4FE7-A1B4-256E7DE21FF2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{B319F6F4-5B26-4633-9938-205A8FCCCA95}"/>
   </bookViews>
   <sheets>
     <sheet name="Investment_Cost" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>PV_plant</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>Average value taken from chart and calculated from $/L to €/MWh using the energy density</t>
+  </si>
+  <si>
+    <t>Power_storage</t>
   </si>
 </sst>
 </file>
@@ -742,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FABD746-4A8E-4371-B5EF-19107F5A398A}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1415,11 +1418,24 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+      <c r="E27" s="4">
+        <v>1</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
       <c r="H27" s="5"/>
       <c r="I27" s="4"/>
     </row>

</xml_diff>